<commit_message>
Re-wrote read_blocks and infer_names to treat row-of rather than row-before as where header/sider are stored
</commit_message>
<xml_diff>
--- a/notes/read_blocks_inference_logic.xlsx
+++ b/notes/read_blocks_inference_logic.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikeb\Documents\Code\growth-curves\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikeb\Documents\Code\gcplyr\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9462C008-BF30-4DAA-8983-0F26E5575A26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30449C35-BBE2-427D-A884-4145F9E68B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{E72C47A2-4044-4009-886A-08FB85B22C14}"/>
+    <workbookView xWindow="-25380" yWindow="3660" windowWidth="14400" windowHeight="7365" activeTab="1" xr2:uid="{E72C47A2-4044-4009-886A-08FB85B22C14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="51">
   <si>
     <t>startrow</t>
   </si>
@@ -127,6 +128,63 @@
   </si>
   <si>
     <t>good</t>
+  </si>
+  <si>
+    <t>header</t>
+  </si>
+  <si>
+    <t>sider</t>
+  </si>
+  <si>
+    <t>output rowname</t>
+  </si>
+  <si>
+    <t>output colname</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>row 1</t>
+  </si>
+  <si>
+    <t>col 1</t>
+  </si>
+  <si>
+    <t>row 1 if [1,1] is empty, otherwise Auto</t>
+  </si>
+  <si>
+    <t>col 1 if [1,1] is empty, otherwise Auto</t>
+  </si>
+  <si>
+    <t>row 1 if [1,startcol] is empty, otherwise Auto</t>
+  </si>
+  <si>
+    <t>startcol if [1,startcol] is empty, otherwise Auto</t>
+  </si>
+  <si>
+    <t>startrow if [startrow,1] is empty, otherwise Auto</t>
+  </si>
+  <si>
+    <t>col 1 if [startrow,1] is empty, otherwise Auto</t>
+  </si>
+  <si>
+    <t>startrow if [startrow,startcol] is empty, otherwise Auto</t>
+  </si>
+  <si>
+    <t>startcol if [startrow,startcol] is empty, otherwise Auto</t>
+  </si>
+  <si>
+    <t>1 if [startrow,1] is empty, otherwise auto</t>
+  </si>
+  <si>
+    <t>1 if [1,1] is empty, otherwise Auto</t>
+  </si>
+  <si>
+    <t>1 if [1,startcol] is empty, otherwise Auto</t>
   </si>
 </sst>
 </file>
@@ -148,7 +206,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,6 +261,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -216,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -227,6 +309,10 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D0E533E-F366-4993-B1A8-0483E1263BE8}">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -991,4 +1077,765 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E79C14F-D8C1-49A7-ACF9-82BE893B8126}">
+  <dimension ref="A1:G37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="47.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s">
+        <v>3</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" t="s">
+        <v>37</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>